<commit_message>
Change to dimensions table
</commit_message>
<xml_diff>
--- a/Tables/dim.xlsx
+++ b/Tables/dim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\KUL\Master thesis\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A6E500-5E39-4D65-9C14-4D4403FC8DF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F0B5FB-8FDF-4593-B7D4-D051DB50F284}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
     <t>f(position):f(strip)</t>
   </si>
   <si>
-    <t>Spatial smoother terms</t>
+    <t>Model components</t>
   </si>
 </sst>
 </file>
@@ -137,21 +137,21 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -471,7 +471,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,54 +489,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="9"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add plot structure to SpATS
</commit_message>
<xml_diff>
--- a/Tables/dim.xlsx
+++ b/Tables/dim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\KUL\Master thesis\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C345BB-276A-43CF-8714-FE702812C1B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DBE1ED-539A-4CA5-880A-F34539AFEACF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,21 +198,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -231,6 +216,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,32 +558,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="9"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -790,28 +790,28 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="5">
         <v>30</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="6">
         <v>21.020583233056751</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6">
         <v>22.584934377586016</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6">
         <v>21.379497107434535</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11">
+      <c r="H8" s="6"/>
+      <c r="I8" s="6">
         <v>22.981437749153994</v>
       </c>
-      <c r="J8" s="11"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -837,12 +837,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -853,7 +853,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,10 +866,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -892,16 +892,16 @@
       <c r="B2">
         <v>6</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -912,16 +912,16 @@
       <c r="B3">
         <v>100</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -932,16 +932,16 @@
       <c r="B4">
         <v>6</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -952,36 +952,36 @@
       <c r="B5">
         <v>100</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="7">
         <v>150</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="12" t="s">
         <v>30</v>
       </c>
     </row>
@@ -990,36 +990,36 @@
         <v>31</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="13">
         <v>459.3</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="13">
         <v>470.2</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="13">
         <v>470.1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="7">
         <v>30</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="9">
         <v>21.020583233056751</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="9">
         <v>22.584934377586016</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="9">
         <v>21.379497107434535</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="9">
         <v>22.981437749153994</v>
       </c>
     </row>

</xml_diff>